<commit_message>
updated js progress report
</commit_message>
<xml_diff>
--- a/JS/ProgressReport.xlsx
+++ b/JS/ProgressReport.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vivek\RoadMap\Interview-Preparation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Interview-Preparation\Interview-Preparation\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A5F3DF-3132-4FE9-A1AC-AE5ECF4B3FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,21 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">JavaScript </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Ghazi's Progress</t>
   </si>
   <si>
     <t>Vivek's Progress</t>
+  </si>
+  <si>
+    <t>JavaScript Progress Report</t>
+  </si>
+  <si>
+    <t>Sr No</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,8 +83,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,147 +374,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>23</v>
       </c>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A1:Q2"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C7:C29 G7:G29">
+      <formula1>"--, in progress, completed"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D29">
+      <formula1>44875</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Progress report for System design
</commit_message>
<xml_diff>
--- a/JS/ProgressReport.xlsx
+++ b/JS/ProgressReport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Ghazi's Progress</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>'</t>
+  </si>
+  <si>
+    <t>Topics</t>
   </si>
 </sst>
 </file>
@@ -88,13 +91,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,12 +381,13 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -393,104 +397,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="3"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -503,10 +510,10 @@
       <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>